<commit_message>
More tests for StringOperators
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/StringOperators.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/StringOperators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="13230"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Issue1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>NONE</t>
   </si>
@@ -28,19 +28,7 @@
     <t>org.openl.rules.binding.StringOperators.*</t>
   </si>
   <si>
-    <t>RETURN</t>
-  </si>
-  <si>
     <t>Steps</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>Result</t>
   </si>
   <si>
     <t>65</t>
@@ -75,9 +63,6 @@
     <t>limit</t>
   </si>
   <si>
-    <t>Limit Age</t>
-  </si>
-  <si>
     <t>= age &lt; limit</t>
   </si>
   <si>
@@ -87,10 +72,124 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Spreadsheet Boolean issue1 (Integer age, LimitAge limit)</t>
-  </si>
-  <si>
     <t>Test issue1</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>gt</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>ge</t>
+  </si>
+  <si>
+    <t>eq</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>= age &gt; limit</t>
+  </si>
+  <si>
+    <t>= age &lt;= limit</t>
+  </si>
+  <si>
+    <t>= age &gt;= limit</t>
+  </si>
+  <si>
+    <t>= age == limit</t>
+  </si>
+  <si>
+    <t>= age != limit</t>
+  </si>
+  <si>
+    <t>= limit &lt; age</t>
+  </si>
+  <si>
+    <t>= limit &gt; age</t>
+  </si>
+  <si>
+    <t>= limit &lt;= age</t>
+  </si>
+  <si>
+    <t>= limit &gt;= age</t>
+  </si>
+  <si>
+    <t>= limit == age</t>
+  </si>
+  <si>
+    <t>= limit != age</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>_res_.$c1$lt</t>
+  </si>
+  <si>
+    <t>_res_.$c1$gt</t>
+  </si>
+  <si>
+    <t>_res_.$c1$le</t>
+  </si>
+  <si>
+    <t>_res_.$c1$ge</t>
+  </si>
+  <si>
+    <t>_res_.$c1$eq</t>
+  </si>
+  <si>
+    <t>_res_.$c1$ne</t>
+  </si>
+  <si>
+    <t>_res_.$c2$lt</t>
+  </si>
+  <si>
+    <t>_res_.$c2$gt</t>
+  </si>
+  <si>
+    <t>_res_.$c2$le</t>
+  </si>
+  <si>
+    <t>_res_.$c2$ge</t>
+  </si>
+  <si>
+    <t>_res_.$c2$eq</t>
+  </si>
+  <si>
+    <t>_res_.$c2$ne</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult issue1 (Integer age, LimitAge limit)</t>
   </si>
 </sst>
 </file>
@@ -214,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -287,17 +386,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -323,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -350,13 +438,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -664,136 +756,492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G15"/>
+  <dimension ref="B3:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C5" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="F9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F10" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="10" t="s">
+      <c r="H10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="F13" s="10">
+        <v>65</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="10">
+        <v>64</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="10">
+        <v>66</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="14">
+        <v>5</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="R16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="14">
+        <v>7</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="R17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="C18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="E13" s="10">
-        <v>65</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="10">
-        <v>64</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="10">
-        <v>66</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="10" t="b">
-        <v>0</v>
+      <c r="C19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>